<commit_message>
added matchup data - week 15 has an error
</commit_message>
<xml_diff>
--- a/standings.xlsx
+++ b/standings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98909D36-C15F-45BC-97A3-51E3DD703F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24745994-D578-4424-B5C2-AD8A0332B618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>Week</t>
-  </si>
-  <si>
-    <t>Leage_Rank</t>
   </si>
   <si>
     <t>Division_Rank</t>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>Boomer Sooners</t>
+  </si>
+  <si>
+    <t>League_Rank</t>
   </si>
 </sst>
 </file>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,15 +451,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48">
         <v>4</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49">
         <v>4</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B50">
         <v>5</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51">
         <v>5</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B52">
         <v>5</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B53">
         <v>5</v>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58">
         <v>5</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B60">
         <v>5</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61">
         <v>5</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B62">
         <v>6</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63">
         <v>6</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B64">
         <v>6</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B65">
         <v>6</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B66">
         <v>6</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B67">
         <v>6</v>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B68">
         <v>6</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B69">
         <v>6</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B70">
         <v>6</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B71">
         <v>6</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72">
         <v>6</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B73">
         <v>6</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B74">
         <v>7</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B75">
         <v>7</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B76">
         <v>7</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B77">
         <v>7</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B78">
         <v>7</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B79">
         <v>7</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B80">
         <v>7</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B81">
         <v>7</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B82">
         <v>7</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B83">
         <v>7</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B84">
         <v>7</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B85">
         <v>7</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B86">
         <v>8</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B87">
         <v>8</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B88">
         <v>8</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B89">
         <v>8</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B90">
         <v>8</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B91">
         <v>8</v>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B92">
         <v>8</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B93">
         <v>8</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B94">
         <v>8</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B95">
         <v>8</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B96">
         <v>8</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B97">
         <v>8</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B98">
         <v>9</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B99">
         <v>9</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B100">
         <v>9</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B101">
         <v>9</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B102">
         <v>9</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B103">
         <v>9</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B104">
         <v>9</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B105">
         <v>9</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B106">
         <v>9</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B107">
         <v>9</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B108">
         <v>9</v>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B109">
         <v>9</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B110">
         <v>10</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B111">
         <v>10</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B112">
         <v>10</v>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B113">
         <v>10</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B114">
         <v>10</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B115">
         <v>10</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B116">
         <v>10</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B117">
         <v>10</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B118">
         <v>10</v>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B119">
         <v>10</v>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B120">
         <v>10</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B121">
         <v>10</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B122">
         <v>11</v>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B123">
         <v>11</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B124">
         <v>11</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B125">
         <v>11</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B126">
         <v>11</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B127">
         <v>11</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B128">
         <v>11</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B129">
         <v>11</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B130">
         <v>11</v>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B131">
         <v>11</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B132">
         <v>11</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B133">
         <v>11</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B134">
         <v>12</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B135">
         <v>12</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B136">
         <v>12</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B137">
         <v>12</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B138">
         <v>12</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B139">
         <v>12</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B140">
         <v>12</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B141">
         <v>12</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B142">
         <v>12</v>
@@ -2433,7 +2433,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B143">
         <v>12</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B144">
         <v>12</v>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B145">
         <v>12</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B146">
         <v>13</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B147">
         <v>13</v>
@@ -2503,7 +2503,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B148">
         <v>13</v>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B149">
         <v>13</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B150">
         <v>13</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B151">
         <v>13</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B152">
         <v>13</v>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B153">
         <v>13</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B154">
         <v>13</v>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B155">
         <v>13</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B156">
         <v>13</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B157">
         <v>13</v>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B158">
         <v>14</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B159">
         <v>14</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B160">
         <v>14</v>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B161">
         <v>14</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B162">
         <v>14</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B163">
         <v>14</v>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B164">
         <v>14</v>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B165">
         <v>14</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B166">
         <v>14</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B167">
         <v>14</v>
@@ -2783,7 +2783,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B168">
         <v>14</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B169">
         <v>14</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B170">
         <v>15</v>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B171">
         <v>15</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B172">
         <v>15</v>
@@ -2853,7 +2853,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B173">
         <v>15</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B174">
         <v>15</v>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B175">
         <v>15</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B176">
         <v>15</v>
@@ -2909,7 +2909,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B177">
         <v>15</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B178">
         <v>15</v>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B179">
         <v>15</v>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B180">
         <v>15</v>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B181">
         <v>15</v>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B182">
         <v>16</v>
@@ -2993,7 +2993,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B183">
         <v>16</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B184">
         <v>16</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B185">
         <v>16</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B186">
         <v>16</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B187">
         <v>16</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B188">
         <v>16</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B189">
         <v>16</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B190">
         <v>16</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B191">
         <v>16</v>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B192">
         <v>16</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B193">
         <v>16</v>

</xml_diff>

<commit_message>
added wk 17 standings, they weren't included in original data
</commit_message>
<xml_diff>
--- a/standings.xlsx
+++ b/standings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24745994-D578-4424-B5C2-AD8A0332B618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F709891F-40BF-4778-B9C8-77CB9FCB545D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="16">
   <si>
     <t>Team</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3145,6 +3145,174 @@
         <v>6</v>
       </c>
     </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>6</v>
+      </c>
+      <c r="B194">
+        <v>17</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>4</v>
+      </c>
+      <c r="B195">
+        <v>17</v>
+      </c>
+      <c r="C195">
+        <v>2</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>11</v>
+      </c>
+      <c r="B196">
+        <v>17</v>
+      </c>
+      <c r="C196">
+        <v>3</v>
+      </c>
+      <c r="D196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>12</v>
+      </c>
+      <c r="B197">
+        <v>17</v>
+      </c>
+      <c r="C197">
+        <v>4</v>
+      </c>
+      <c r="D197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198">
+        <v>17</v>
+      </c>
+      <c r="C198">
+        <v>5</v>
+      </c>
+      <c r="D198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>7</v>
+      </c>
+      <c r="B199">
+        <v>17</v>
+      </c>
+      <c r="C199">
+        <v>6</v>
+      </c>
+      <c r="D199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>8</v>
+      </c>
+      <c r="B200">
+        <v>17</v>
+      </c>
+      <c r="C200">
+        <v>7</v>
+      </c>
+      <c r="D200">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>9</v>
+      </c>
+      <c r="B201">
+        <v>17</v>
+      </c>
+      <c r="C201">
+        <v>8</v>
+      </c>
+      <c r="D201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>13</v>
+      </c>
+      <c r="B202">
+        <v>17</v>
+      </c>
+      <c r="C202">
+        <v>9</v>
+      </c>
+      <c r="D202">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>5</v>
+      </c>
+      <c r="B203">
+        <v>17</v>
+      </c>
+      <c r="C203">
+        <v>10</v>
+      </c>
+      <c r="D203">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>14</v>
+      </c>
+      <c r="B204">
+        <v>17</v>
+      </c>
+      <c r="C204">
+        <v>11</v>
+      </c>
+      <c r="D204">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>10</v>
+      </c>
+      <c r="B205">
+        <v>17</v>
+      </c>
+      <c r="C205">
+        <v>12</v>
+      </c>
+      <c r="D205">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>